<commit_message>
added efficient frontier graph and VaR CVaR calculation
</commit_message>
<xml_diff>
--- a/Portfolio-ICMarketsDemo.xlsx
+++ b/Portfolio-ICMarketsDemo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="444" documentId="8_{76DEAA88-E9EE-482A-9643-029D2D45417D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{884C3BF8-9E31-482E-8C9F-01EAF0566225}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USD_Prices" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,11 @@
     <sheet name="MaxSharpe_Portfolio" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -262,43 +265,121 @@
     <t>contribution_ret</t>
   </si>
   <si>
-    <t>symbol</t>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial </t>
   </si>
   <si>
     <t>asset</t>
   </si>
   <si>
+    <t>symbol</t>
+  </si>
+  <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>market_value</t>
+  </si>
+  <si>
+    <t>last price (USD normalized)</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>broker-level lots sizing</t>
+  </si>
+  <si>
+    <t>broker-level position</t>
+  </si>
+  <si>
+    <t>mu_annual projection</t>
   </si>
   <si>
     <t>Turkish Lira</t>
   </si>
   <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>TRY</t>
+  </si>
+  <si>
+    <t>Polish Zloty</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
     <t>Euro</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
   <si>
     <t>Canadian Dollar</t>
   </si>
   <si>
+    <t>CAD</t>
+  </si>
+  <si>
     <t>Sout African Rand</t>
+  </si>
+  <si>
+    <t>ZAR</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
   <si>
     <t>Thai Baht</t>
   </si>
   <si>
+    <t>THB</t>
+  </si>
+  <si>
     <t>Swedish Krona</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>Dow Jones 30</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Contracts</t>
   </si>
   <si>
     <t>US 30Y T-Bills</t>
   </si>
   <si>
-    <t>Dow Jones 30</t>
+    <t>Bonds</t>
+  </si>
+  <si>
+    <t>bills</t>
   </si>
   <si>
     <t>South Africa 40</t>
   </si>
   <si>
     <t>Gold</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>t oz</t>
   </si>
   <si>
     <t>Canada 60</t>
@@ -310,7 +391,13 @@
     <t>Japanese Yen</t>
   </si>
   <si>
+    <t>JPY</t>
+  </si>
+  <si>
     <t>New Zealand Dollar</t>
+  </si>
+  <si>
+    <t>NZD</t>
   </si>
   <si>
     <t>Volatility Index</t>
@@ -322,85 +409,22 @@
     <t>Solana</t>
   </si>
   <si>
+    <t>Crypto</t>
+  </si>
+  <si>
+    <t>sol</t>
+  </si>
+  <si>
     <t>West Texas Intermediate</t>
+  </si>
+  <si>
+    <t>bbl</t>
   </si>
   <si>
     <t>Australian Dollar</t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Bonds</t>
-  </si>
-  <si>
-    <t>Commodity</t>
-  </si>
-  <si>
-    <t>Crypto</t>
-  </si>
-  <si>
-    <t>Polish Zloty</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>t oz</t>
-  </si>
-  <si>
-    <t>bbl</t>
-  </si>
-  <si>
-    <t>bills</t>
-  </si>
-  <si>
-    <t>sol</t>
-  </si>
-  <si>
-    <t>TRY</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>ZAR</t>
-  </si>
-  <si>
-    <t>THB</t>
-  </si>
-  <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
     <t>AUD</t>
-  </si>
-  <si>
-    <t>Contracts</t>
-  </si>
-  <si>
-    <t>broker-level lots sizing</t>
-  </si>
-  <si>
-    <t>last price (USD normalized)</t>
   </si>
   <si>
     <t>LOOKBACK_DAYS = 60         # lookback (trading days) used to compute returns</t>
@@ -414,27 +438,6 @@
   <si>
     <t>ALLOW_SHORTS = False           # set True to allow negative weights</t>
   </si>
-  <si>
-    <t>mu_annual projection</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>broker-level position</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial </t>
-  </si>
-  <si>
-    <t>market_value</t>
-  </si>
 </sst>
 </file>
 
@@ -446,7 +449,7 @@
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,10 +625,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -917,12 +916,12 @@
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71">
       <c r="A2" s="2">
         <v>45887</v>
       </c>
@@ -1352,7 +1351,7 @@
         <v>0.82250000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71">
       <c r="A3" s="2">
         <v>45888</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>0.79261000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71">
       <c r="A4" s="2">
         <v>45889</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>0.82004999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71">
       <c r="A5" s="2">
         <v>45890</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>0.80159999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71">
       <c r="A6" s="2">
         <v>45891</v>
       </c>
@@ -2212,7 +2211,7 @@
         <v>0.86250000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71">
       <c r="A7" s="2">
         <v>45895</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>0.79381000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:71">
       <c r="A8" s="2">
         <v>45896</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>0.79651000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:71">
       <c r="A9" s="2">
         <v>45897</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>0.77627999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71">
       <c r="A10" s="2">
         <v>45898</v>
       </c>
@@ -3072,7 +3071,7 @@
         <v>0.72621000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71">
       <c r="A11" s="2">
         <v>45902</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>0.72441</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71">
       <c r="A12" s="2">
         <v>45903</v>
       </c>
@@ -3502,7 +3501,7 @@
         <v>0.73231000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71">
       <c r="A13" s="2">
         <v>45904</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>0.70601000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71">
       <c r="A14" s="2">
         <v>45905</v>
       </c>
@@ -3932,7 +3931,7 @@
         <v>0.71891000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71">
       <c r="A15" s="2">
         <v>45908</v>
       </c>
@@ -4147,7 +4146,7 @@
         <v>0.71650999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71">
       <c r="A16" s="2">
         <v>45909</v>
       </c>
@@ -4362,7 +4361,7 @@
         <v>0.72221000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71">
       <c r="A17" s="2">
         <v>45910</v>
       </c>
@@ -4577,7 +4576,7 @@
         <v>0.73165999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71">
       <c r="A18" s="2">
         <v>45911</v>
       </c>
@@ -4792,7 +4791,7 @@
         <v>0.74480999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71">
       <c r="A19" s="2">
         <v>45912</v>
       </c>
@@ -5007,7 +5006,7 @@
         <v>0.77059999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71">
       <c r="A20" s="2">
         <v>45915</v>
       </c>
@@ -5222,7 +5221,7 @@
         <v>0.75619999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71">
       <c r="A21" s="2">
         <v>45916</v>
       </c>
@@ -5437,7 +5436,7 @@
         <v>0.76970000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71">
       <c r="A22" s="2">
         <v>45917</v>
       </c>
@@ -5652,7 +5651,7 @@
         <v>0.77059999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71">
       <c r="A23" s="2">
         <v>45918</v>
       </c>
@@ -5867,7 +5866,7 @@
         <v>0.7954</v>
       </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71">
       <c r="A24" s="2">
         <v>45919</v>
       </c>
@@ -6082,7 +6081,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71">
       <c r="A25" s="2">
         <v>45922</v>
       </c>
@@ -6297,7 +6296,7 @@
         <v>0.69740000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71">
       <c r="A26" s="2">
         <v>45923</v>
       </c>
@@ -6512,7 +6511,7 @@
         <v>0.69569999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71">
       <c r="A27" s="2">
         <v>45925</v>
       </c>
@@ -6727,7 +6726,7 @@
         <v>0.65339999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71">
       <c r="A28" s="2">
         <v>45926</v>
       </c>
@@ -6942,7 +6941,7 @@
         <v>0.67330000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71">
       <c r="A29" s="2">
         <v>45929</v>
       </c>
@@ -7157,7 +7156,7 @@
         <v>0.67049999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71">
       <c r="A30" s="2">
         <v>45930</v>
       </c>
@@ -7372,7 +7371,7 @@
         <v>0.66649999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71">
       <c r="A31" s="2">
         <v>45932</v>
       </c>
@@ -7587,7 +7586,7 @@
         <v>0.70650000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71">
       <c r="A32" s="2">
         <v>45933</v>
       </c>
@@ -7802,7 +7801,7 @@
         <v>0.71750000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:71">
       <c r="A33" s="2">
         <v>45936</v>
       </c>
@@ -8017,7 +8016,7 @@
         <v>0.72050000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:71">
       <c r="A34" s="2">
         <v>45938</v>
       </c>
@@ -8232,7 +8231,7 @@
         <v>0.6845</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:71">
       <c r="A35" s="2">
         <v>45939</v>
       </c>
@@ -8447,7 +8446,7 @@
         <v>0.66649999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:71">
       <c r="A36" s="2">
         <v>45940</v>
       </c>
@@ -8675,12 +8674,12 @@
       <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8895,7 +8894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71">
       <c r="A2" s="2">
         <v>45888</v>
       </c>
@@ -9110,7 +9109,7 @@
         <v>-3.7017185258265473E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71">
       <c r="A3" s="2">
         <v>45889</v>
       </c>
@@ -9325,7 +9324,7 @@
         <v>3.4034016627856413E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71">
       <c r="A4" s="2">
         <v>45890</v>
       </c>
@@ -9540,7 +9539,7 @@
         <v>-2.2755583678517599E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71">
       <c r="A5" s="2">
         <v>45891</v>
       </c>
@@ -9755,7 +9754,7 @@
         <v>7.3225418574914547E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71">
       <c r="A6" s="2">
         <v>45895</v>
       </c>
@@ -9970,7 +9969,7 @@
         <v>-8.2991011004254073E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71">
       <c r="A7" s="2">
         <v>45896</v>
       </c>
@@ -10185,7 +10184,7 @@
         <v>3.395546297839197E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:71">
       <c r="A8" s="2">
         <v>45897</v>
       </c>
@@ -10400,7 +10399,7 @@
         <v>-2.5726404355205679E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:71">
       <c r="A9" s="2">
         <v>45898</v>
       </c>
@@ -10615,7 +10614,7 @@
         <v>-6.6674050647259675E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71">
       <c r="A10" s="2">
         <v>45902</v>
       </c>
@@ -10830,7 +10829,7 @@
         <v>-2.481698754772776E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71">
       <c r="A11" s="2">
         <v>45903</v>
       </c>
@@ -11045,7 +11044,7 @@
         <v>1.0846391137551431E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71">
       <c r="A12" s="2">
         <v>45904</v>
       </c>
@@ -11260,7 +11259,7 @@
         <v>-3.6574519880535013E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71">
       <c r="A13" s="2">
         <v>45905</v>
       </c>
@@ -11475,7 +11474,7 @@
         <v>1.8106774334694931E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71">
       <c r="A14" s="2">
         <v>45908</v>
       </c>
@@ -11690,7 +11689,7 @@
         <v>-3.3439721286167572E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71">
       <c r="A15" s="2">
         <v>45909</v>
       </c>
@@ -11905,7 +11904,7 @@
         <v>7.9237514224327343E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71">
       <c r="A16" s="2">
         <v>45910</v>
       </c>
@@ -12120,7 +12119,7 @@
         <v>1.2999969854949721E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71">
       <c r="A17" s="2">
         <v>45911</v>
       </c>
@@ -12335,7 +12334,7 @@
         <v>1.7813227113585631E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71">
       <c r="A18" s="2">
         <v>45912</v>
       </c>
@@ -12550,7 +12549,7 @@
         <v>3.4040279896132619E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71">
       <c r="A19" s="2">
         <v>45915</v>
       </c>
@@ -12765,7 +12764,7 @@
         <v>-1.8863540735224671E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71">
       <c r="A20" s="2">
         <v>45916</v>
       </c>
@@ -12980,7 +12979,7 @@
         <v>1.7694937083439329E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71">
       <c r="A21" s="2">
         <v>45917</v>
       </c>
@@ -13195,7 +13194,7 @@
         <v>1.168603651785338E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71">
       <c r="A22" s="2">
         <v>45918</v>
       </c>
@@ -13410,7 +13409,7 @@
         <v>3.1675700581533101E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71">
       <c r="A23" s="2">
         <v>45919</v>
       </c>
@@ -13625,7 +13624,7 @@
         <v>-5.2127383524565557E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71">
       <c r="A24" s="2">
         <v>45922</v>
       </c>
@@ -13840,7 +13839,7 @@
         <v>-7.9358615007473876E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71">
       <c r="A25" s="2">
         <v>45923</v>
       </c>
@@ -14055,7 +14054,7 @@
         <v>-2.440601311955171E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71">
       <c r="A26" s="2">
         <v>45925</v>
       </c>
@@ -14270,7 +14269,7 @@
         <v>-6.2729033762625896E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71">
       <c r="A27" s="2">
         <v>45926</v>
       </c>
@@ -14485,7 +14484,7 @@
         <v>3.0001496384265469E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71">
       <c r="A28" s="2">
         <v>45929</v>
       </c>
@@ -14700,7 +14699,7 @@
         <v>-4.1672928295020117E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71">
       <c r="A29" s="2">
         <v>45930</v>
       </c>
@@ -14915,7 +14914,7 @@
         <v>-5.9835631029698799E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71">
       <c r="A30" s="2">
         <v>45932</v>
       </c>
@@ -15130,7 +15129,7 @@
         <v>5.8283062505818828E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71">
       <c r="A31" s="2">
         <v>45933</v>
       </c>
@@ -15345,7 +15344,7 @@
         <v>1.544974550919403E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71">
       <c r="A32" s="2">
         <v>45936</v>
       </c>
@@ -15560,7 +15559,7 @@
         <v>4.1724678058006059E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:71">
       <c r="A33" s="2">
         <v>45938</v>
       </c>
@@ -15775,7 +15774,7 @@
         <v>-5.1256770711073207E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:71">
       <c r="A34" s="2">
         <v>45939</v>
       </c>
@@ -15990,7 +15989,7 @@
         <v>-2.6648505109740261E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:71">
       <c r="A35" s="2">
         <v>45940</v>
       </c>
@@ -16216,14 +16215,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -16231,7 +16230,7 @@
         <v>-1.4093385340218969</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -16239,7 +16238,7 @@
         <v>-4.7348962621082152E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -16247,7 +16246,7 @@
         <v>-4.796520875108419E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -16255,7 +16254,7 @@
         <v>0.72708635245033193</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -16263,7 +16262,7 @@
         <v>-0.22308024917005589</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -16271,7 +16270,7 @@
         <v>2.681118232436285</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -16279,7 +16278,7 @@
         <v>-6.4687694258045353E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -16287,7 +16286,7 @@
         <v>0.33814291738023478</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -16295,7 +16294,7 @@
         <v>-5.3461179594938353E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -16303,7 +16302,7 @@
         <v>0.1408929617376577</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -16311,7 +16310,7 @@
         <v>-0.10475493889823929</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -16319,7 +16318,7 @@
         <v>4.6226353491704973E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -16327,7 +16326,7 @@
         <v>6.5044107096713627E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -16335,7 +16334,7 @@
         <v>-0.74005302962692876</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -16343,7 +16342,7 @@
         <v>-4.6854742239782268E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -16351,7 +16350,7 @@
         <v>-1.7009059045684359E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -16359,7 +16358,7 @@
         <v>-0.1702540137020313</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -16367,7 +16366,7 @@
         <v>-3.239281583481775</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -16375,7 +16374,7 @@
         <v>-5.1716542425168648E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -16383,7 +16382,7 @@
         <v>-0.1505459544210534</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -16391,7 +16390,7 @@
         <v>8.6176162753889337E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -16399,7 +16398,7 @@
         <v>0.23377432983314919</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -16407,7 +16406,7 @@
         <v>-0.56265162386895118</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -16415,7 +16414,7 @@
         <v>-1.6356947887441959</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -16423,7 +16422,7 @@
         <v>0.42634927009440932</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -16431,7 +16430,7 @@
         <v>-0.1989966897769653</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -16439,7 +16438,7 @@
         <v>0.28274487061622011</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -16447,7 +16446,7 @@
         <v>0.17292298815613161</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -16455,7 +16454,7 @@
         <v>-0.52200112412190436</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -16463,7 +16462,7 @@
         <v>-0.86513285663681239</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -16471,7 +16470,7 @@
         <v>0.69672677572401154</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -16479,7 +16478,7 @@
         <v>0.28600943912934962</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -16487,7 +16486,7 @@
         <v>0.7937672085462244</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -16495,7 +16494,7 @@
         <v>8.8620276172037563E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -16503,7 +16502,7 @@
         <v>0.32318965383903631</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -16511,7 +16510,7 @@
         <v>-0.27280747563229052</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -16519,7 +16518,7 @@
         <v>0.16306228462160191</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -16527,7 +16526,7 @@
         <v>3.9946911921136842E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -16535,7 +16534,7 @@
         <v>-2.8188539783556079</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -16543,7 +16542,7 @@
         <v>0.23955868647164549</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -16551,7 +16550,7 @@
         <v>5.3609648495082783E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -16559,7 +16558,7 @@
         <v>6.9002499569791306E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -16567,7 +16566,7 @@
         <v>0.10546216884767901</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -16575,7 +16574,7 @@
         <v>-7.8018810300400782E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -16583,7 +16582,7 @@
         <v>-4.1373367856297791E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -16591,7 +16590,7 @@
         <v>-2.837581596960604E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -16599,7 +16598,7 @@
         <v>2.5527416337711981E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -16607,7 +16606,7 @@
         <v>-3.718969231747097E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -16615,7 +16614,7 @@
         <v>-3.5433749558041058E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -16623,7 +16622,7 @@
         <v>0.1661156635269419</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -16631,7 +16630,7 @@
         <v>-7.1049279899897816E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -16639,7 +16638,7 @@
         <v>-7.1209778416239544E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -16647,7 +16646,7 @@
         <v>3.9971460513471987E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -16655,7 +16654,7 @@
         <v>-5.0994709677884817E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -16663,7 +16662,7 @@
         <v>6.8823162202848426E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -16671,7 +16670,7 @@
         <v>2.8696027516965181E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -16679,7 +16678,7 @@
         <v>0.17480417157926101</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -16687,7 +16686,7 @@
         <v>-4.8554465637608367E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -16695,7 +16694,7 @@
         <v>0.1143398356132389</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -16703,7 +16702,7 @@
         <v>0.2816266628460079</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -16711,7 +16710,7 @@
         <v>9.2142285246401862E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -16719,7 +16718,7 @@
         <v>1.114721475751983</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -16727,7 +16726,7 @@
         <v>4.0545788563280416</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -16735,7 +16734,7 @@
         <v>2.7513324892962752</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -16743,7 +16742,7 @@
         <v>-1.201439954677809</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -16751,7 +16750,7 @@
         <v>3.24368626465944</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -16759,7 +16758,7 @@
         <v>2.651156819220827</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -16767,7 +16766,7 @@
         <v>-1.1093900998992241</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -16775,7 +16774,7 @@
         <v>-1.231947239409851</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -16794,9 +16793,9 @@
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -17008,7 +17007,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -17223,7 +17222,7 @@
         <v>0.37521211942129712</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -17438,7 +17437,7 @@
         <v>3.716271550041219E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -17653,7 +17652,7 @@
         <v>1.060001673218384E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -17868,7 +17867,7 @@
         <v>0.36628487158817652</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -18083,7 +18082,7 @@
         <v>0.31382888976085521</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -18298,7 +18297,7 @@
         <v>0.19900365485755639</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:71">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -18513,7 +18512,7 @@
         <v>0.19287238121232059</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:71">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -18728,7 +18727,7 @@
         <v>2.0088193826376079E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -18943,7 +18942,7 @@
         <v>2.153108149504997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -19158,7 +19157,7 @@
         <v>0.46221337872962331</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -19373,7 +19372,7 @@
         <v>0.35413251573299409</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -19588,7 +19587,7 @@
         <v>-1.7921888368813321E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -19803,7 +19802,7 @@
         <v>2.3389687041218889E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -20018,7 +20017,7 @@
         <v>0.38539235915117398</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -20233,7 +20232,7 @@
         <v>3.5230992394221637E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -20448,7 +20447,7 @@
         <v>4.3510570345317509E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -20663,7 +20662,7 @@
         <v>3.4993668875262618E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -20878,7 +20877,7 @@
         <v>0.37835034329099421</v>
       </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -21093,7 +21092,7 @@
         <v>5.4164548879967522E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -21308,7 +21307,7 @@
         <v>2.0573539714497189E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -21523,7 +21522,7 @@
         <v>2.9447112174355639E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -21738,7 +21737,7 @@
         <v>5.6183605981077127E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -21953,7 +21952,7 @@
         <v>0.40542412755535928</v>
       </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -22168,7 +22167,7 @@
         <v>0.41183002043404848</v>
       </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -22383,7 +22382,7 @@
         <v>0.27352387195632771</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -22598,7 +22597,7 @@
         <v>5.0055948451533147E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -22813,7 +22812,7 @@
         <v>4.7428284225846683E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -23028,7 +23027,7 @@
         <v>4.2396002589250019E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -23243,7 +23242,7 @@
         <v>3.2147298339667632E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -23458,7 +23457,7 @@
         <v>0.26747700712981409</v>
       </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -23673,7 +23672,7 @@
         <v>6.2616622229952401E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:71">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -23888,7 +23887,7 @@
         <v>6.2029745321682338E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:71">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -24103,7 +24102,7 @@
         <v>0.37674577470376258</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:71">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -24318,7 +24317,7 @@
         <v>3.7002629553918448E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:71">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -24533,7 +24532,7 @@
         <v>3.7797129727469722E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:71">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -24748,7 +24747,7 @@
         <v>5.5030277500781703E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:71">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -24963,7 +24962,7 @@
         <v>1.520932531095345E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:71">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -25178,7 +25177,7 @@
         <v>7.4690041306486477E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:71">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -25393,7 +25392,7 @@
         <v>0.4655800368585471</v>
       </c>
     </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:71">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -25608,7 +25607,7 @@
         <v>6.6551954751894737E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:71">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -25823,7 +25822,7 @@
         <v>2.9559772019294588E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:71">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -26038,7 +26037,7 @@
         <v>2.9419331681105471E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:71">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -26253,7 +26252,7 @@
         <v>-7.6565584973237082E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:71">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -26468,7 +26467,7 @@
         <v>-1.497675659431571E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:71">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -26683,7 +26682,7 @@
         <v>-1.7975363578407581E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:71">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -26898,7 +26897,7 @@
         <v>-2.1442238518166661E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:71">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -27113,7 +27112,7 @@
         <v>-1.7901045300543379E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:71">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -27328,7 +27327,7 @@
         <v>1.635205775049991E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:71">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -27543,7 +27542,7 @@
         <v>-2.707646243615305E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:71">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -27758,7 +27757,7 @@
         <v>-1.6512347270560241E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:71">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -27973,7 +27972,7 @@
         <v>-1.8867432473959202E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:71">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -28188,7 +28187,7 @@
         <v>-3.1758335811779913E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:71">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -28403,7 +28402,7 @@
         <v>-1.7615398769385358E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:71">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -28618,7 +28617,7 @@
         <v>-2.333652199209614E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:71">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -28833,7 +28832,7 @@
         <v>-1.015533359329907E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:71">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -29048,7 +29047,7 @@
         <v>-1.0818801822925869E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:71">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -29263,7 +29262,7 @@
         <v>-3.9102938556777617E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:71">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -29478,7 +29477,7 @@
         <v>-3.1534349111232797E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:71">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -29693,7 +29692,7 @@
         <v>4.97125396577536E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:71">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -29908,7 +29907,7 @@
         <v>1.1088734953122461E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:71">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -30123,7 +30122,7 @@
         <v>3.6856578561134737E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:71">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -30338,7 +30337,7 @@
         <v>-0.16214672188105861</v>
       </c>
     </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:71">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -30553,7 +30552,7 @@
         <v>-4.6838294146596708E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:71">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -30768,7 +30767,7 @@
         <v>-1.589281970714564E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:71">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -30983,7 +30982,7 @@
         <v>0.34220109258896619</v>
       </c>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:71">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -31198,7 +31197,7 @@
         <v>-3.3657261129512638E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:71">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -31413,7 +31412,7 @@
         <v>3.9538631642192033E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:71">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -31628,7 +31627,7 @@
         <v>0.2682140757124587</v>
       </c>
     </row>
-    <row r="70" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:71">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -31843,7 +31842,7 @@
         <v>2.077464466157284E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:71">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -32071,14 +32070,14 @@
       <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
@@ -32089,7 +32088,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -32103,7 +32102,7 @@
         <v>4.0572048223546489</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -32117,7 +32116,7 @@
         <v>0.53241985403944692</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -32131,7 +32130,7 @@
         <v>-0.61239148107395425</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -32145,7 +32144,7 @@
         <v>1.3478065178733369</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -32159,7 +32158,7 @@
         <v>-0.36949948350219969</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -32173,7 +32172,7 @@
         <v>0.17734145005484481</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -32187,7 +32186,7 @@
         <v>-0.28302063871226069</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -32201,7 +32200,7 @@
         <v>0.2530375408967907</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -32215,7 +32214,7 @@
         <v>1.044834919158689</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -32229,7 +32228,7 @@
         <v>1.135664644430139</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>64</v>
       </c>
@@ -32243,7 +32242,7 @@
         <v>4.1269987339444132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -32257,7 +32256,7 @@
         <v>0.46663722598472401</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -32271,7 +32270,7 @@
         <v>8.5563099466541226E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -32285,7 +32284,7 @@
         <v>0.20266110950286911</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -32299,7 +32298,7 @@
         <v>-0.56376121405165669</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -32313,7 +32312,7 @@
         <v>0.5573607378759915</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
@@ -32327,7 +32326,7 @@
         <v>1.6218315425312171</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -32341,7 +32340,7 @@
         <v>0.26194317882025409</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
@@ -32355,7 +32354,7 @@
         <v>-0.35726469942885658</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -32369,7 +32368,7 @@
         <v>-1.278421990769218E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -32383,7 +32382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -32397,7 +32396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -32411,7 +32410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -32425,7 +32424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -32439,7 +32438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -32453,7 +32452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -32467,7 +32466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -32481,7 +32480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -32495,7 +32494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -32509,7 +32508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -32523,7 +32522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -32537,7 +32536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -32551,7 +32550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -32565,7 +32564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -32579,7 +32578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -32593,7 +32592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -32607,7 +32606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -32621,7 +32620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>22</v>
       </c>
@@ -32635,7 +32634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
@@ -32649,7 +32648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -32663,7 +32662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -32677,7 +32676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
@@ -32691,7 +32690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -32705,7 +32704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>28</v>
       </c>
@@ -32719,7 +32718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -32733,7 +32732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>32</v>
       </c>
@@ -32747,7 +32746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>34</v>
       </c>
@@ -32761,7 +32760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>35</v>
       </c>
@@ -32775,7 +32774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
@@ -32789,7 +32788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
@@ -32803,7 +32802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>38</v>
       </c>
@@ -32817,7 +32816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>39</v>
       </c>
@@ -32831,7 +32830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
@@ -32845,7 +32844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>44</v>
       </c>
@@ -32859,7 +32858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
@@ -32873,7 +32872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
@@ -32887,7 +32886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
@@ -32901,7 +32900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
@@ -32915,7 +32914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>49</v>
       </c>
@@ -32929,7 +32928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>51</v>
       </c>
@@ -32943,7 +32942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>52</v>
       </c>
@@ -32957,7 +32956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>55</v>
       </c>
@@ -32971,7 +32970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>59</v>
       </c>
@@ -32985,7 +32984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
         <v>61</v>
       </c>
@@ -32999,7 +32998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -33013,7 +33012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
@@ -33027,7 +33026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -33041,7 +33040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -33055,7 +33054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -33085,7 +33084,7 @@
       <selection activeCell="C3" sqref="C3:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -33103,56 +33102,56 @@
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="B1" s="19">
         <v>45943</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="F1" s="6">
         <v>100000</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>72</v>
@@ -33161,9 +33160,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>57</v>
@@ -33172,7 +33171,7 @@
         <v>0.1652012897918369</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E3" s="17">
         <f t="shared" ref="E3:E22" si="0">C3*$F$1</f>
@@ -33186,7 +33185,7 @@
         <v>690929.69381780387</v>
       </c>
       <c r="H3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="I3" s="21">
         <f t="shared" ref="I3:I9" si="2">E3/100000</f>
@@ -33197,7 +33196,7 @@
         <v>0.17480417157926101</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>57</v>
@@ -33216,9 +33215,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>53</v>
@@ -33227,7 +33226,7 @@
         <v>8.8017010913861105E-2</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E4" s="17">
         <f t="shared" si="0"/>
@@ -33241,20 +33240,20 @@
         <v>32343.974495039507</v>
       </c>
       <c r="H4" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="I4" s="21">
         <f t="shared" si="2"/>
         <v>8.8017010913861105E-2</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K4" s="5">
         <v>3.9971460513471987E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>53</v>
@@ -33273,9 +33272,9 @@
         <v>0.17343750000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>15</v>
@@ -33284,7 +33283,7 @@
         <v>0.21742762529982601</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E5" s="17">
         <f t="shared" si="0"/>
@@ -33298,20 +33297,20 @@
         <v>18739.883584415809</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="I5" s="21">
         <f t="shared" si="2"/>
         <v>0.21742762529982598</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K5" s="5">
         <v>-4.6854742239782268E-2</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>15</v>
@@ -33330,9 +33329,9 @@
         <v>0.17018229166666668</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>43</v>
@@ -33341,7 +33340,7 @@
         <v>0.52879127740992216</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E6" s="17">
         <f t="shared" si="0"/>
@@ -33355,20 +33354,20 @@
         <v>74016.242047450985</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="I6" s="21">
         <f t="shared" si="2"/>
         <v>0.52879127740992216</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K6" s="5">
         <v>0.10546216884767901</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>43</v>
@@ -33387,9 +33386,9 @@
         <v>0.16640625000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>58</v>
@@ -33398,7 +33397,7 @@
         <v>5.6279658455404011E-4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E7" s="17">
         <f t="shared" si="0"/>
@@ -33412,20 +33411,20 @@
         <v>980.15741227475246</v>
       </c>
       <c r="H7" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I7" s="21">
         <f t="shared" si="2"/>
         <v>5.6279658455404011E-4</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K7" s="5">
         <v>-4.8554465637608367E-2</v>
       </c>
       <c r="L7" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>58</v>
@@ -33444,15 +33443,15 @@
         <v>9.9088541666666669E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E8" s="17">
         <f t="shared" si="0"/>
@@ -33466,20 +33465,20 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="I8" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K8" s="5">
         <v>2.8696027516965181E-2</v>
       </c>
       <c r="L8" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>56</v>
@@ -33498,15 +33497,15 @@
         <v>8.0468750000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E9" s="17">
         <f t="shared" si="0"/>
@@ -33520,20 +33519,20 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="I9" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K9" s="5">
         <v>-5.0994709677884817E-2</v>
       </c>
       <c r="L9" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>54</v>
@@ -33552,15 +33551,15 @@
         <v>7.2265625E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E10" s="8">
         <f t="shared" si="0"/>
@@ -33574,20 +33573,20 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="I10" s="20">
         <f>G10</f>
         <v>0</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K10" s="5">
         <v>5.3609648495082783E-2</v>
       </c>
       <c r="L10" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>41</v>
@@ -33606,15 +33605,15 @@
         <v>6.145833333333333E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E11" s="8">
         <f t="shared" si="0"/>
@@ -33628,20 +33627,20 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I11" s="20">
         <f>G11/100</f>
         <v>0</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K11" s="5">
         <v>0.2816266628460079</v>
       </c>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>60</v>
@@ -33660,15 +33659,15 @@
         <v>4.8307291666666669E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="0"/>
@@ -33682,20 +33681,20 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="I12" s="20">
         <f>G12</f>
         <v>0</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K12" s="5">
         <v>0.69672677572401154</v>
       </c>
       <c r="L12" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>31</v>
@@ -33714,15 +33713,15 @@
         <v>2.1223958333333334E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" si="0"/>
@@ -33736,20 +33735,20 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="I13" s="22">
         <f>G13/100</f>
         <v>0</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K13" s="5">
         <v>2.7513324892962752</v>
       </c>
       <c r="L13" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>64</v>
@@ -33768,15 +33767,15 @@
         <v>1.953125E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E14" s="8">
         <f t="shared" si="0"/>
@@ -33790,20 +33789,20 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="I14" s="23">
         <f>G14</f>
         <v>0</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K14" s="5">
         <v>0.33814291738023478</v>
       </c>
       <c r="L14" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>8</v>
@@ -33822,15 +33821,15 @@
         <v>1.7968749999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" si="0"/>
@@ -33844,20 +33843,20 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="I15" s="20">
         <f>G15</f>
         <v>0</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K15" s="5">
         <v>6.9002499569791306E-2</v>
       </c>
       <c r="L15" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>42</v>
@@ -33876,15 +33875,15 @@
         <v>1.6145833333333335E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E16" s="17">
         <f t="shared" si="0"/>
@@ -33898,20 +33897,20 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I16" s="21">
         <f>E16/100000</f>
         <v>0</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K16" s="5">
         <v>0.1661156635269419</v>
       </c>
       <c r="L16" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>50</v>
@@ -33930,15 +33929,15 @@
         <v>1.5885416666666666E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E17" s="18">
         <f t="shared" si="0"/>
@@ -33952,20 +33951,20 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I17" s="21">
         <f>G17/100000</f>
         <v>0</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K17" s="5">
         <v>-0.52200112412190436</v>
       </c>
       <c r="L17" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>29</v>
@@ -33984,15 +33983,15 @@
         <v>1.4062500000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" si="0"/>
@@ -34006,20 +34005,20 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="I18" s="20">
         <f>G18</f>
         <v>0</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K18" s="5">
         <v>1.114721475751983</v>
       </c>
       <c r="L18" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>62</v>
@@ -34038,15 +34037,15 @@
         <v>6.510416666666667E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
         <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E19" s="8">
         <f t="shared" si="0"/>
@@ -34060,20 +34059,20 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="I19" s="22">
         <f>G19/1000</f>
         <v>0</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K19" s="5">
         <v>4.0545788563280416</v>
       </c>
       <c r="L19" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>63</v>
@@ -34092,15 +34091,15 @@
         <v>5.2083333333333339E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="0"/>
@@ -34114,20 +34113,20 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="I20" s="20">
         <f>G20</f>
         <v>0</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="K20" s="5">
         <v>0.7937672085462244</v>
       </c>
       <c r="L20" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>33</v>
@@ -34146,15 +34145,15 @@
         <v>4.2968750000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
         <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E21" s="8">
         <f t="shared" si="0"/>
@@ -34168,20 +34167,20 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="I21" s="22">
         <f>G21/100</f>
         <v>0</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K21" s="5">
         <v>-1.231947239409851</v>
       </c>
       <c r="L21" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>69</v>
@@ -34200,15 +34199,15 @@
         <v>3.7760416666666667E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E22" s="18">
         <f t="shared" si="0"/>
@@ -34222,20 +34221,20 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="I22" s="21">
         <f>G22/100000</f>
         <v>0</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="K22" s="5">
         <v>-4.7348962621082152E-2</v>
       </c>
       <c r="L22" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>2</v>
@@ -34254,22 +34253,22 @@
         <v>3.7760416666666667E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="C23" s="4"/>
       <c r="N23">
         <f>SUM(N3:N22)</f>
         <v>76.8</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E26"/>
       <c r="F26" s="1" t="s">
@@ -34279,9 +34278,9 @@
         <v>0.26634097876205137</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E27"/>
       <c r="F27" s="1" t="s">
@@ -34291,9 +34290,9 @@
         <v>0.23799992797719449</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E28"/>
       <c r="F28" s="1" t="s">
@@ -34303,7 +34302,7 @@
         <v>0.2045057572135823</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18">
       <c r="F29" s="1" t="s">
         <v>60</v>
       </c>
@@ -34311,7 +34310,7 @@
         <v>0.13840293137436749</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18">
       <c r="F30" s="1" t="s">
         <v>64</v>
       </c>
@@ -34319,7 +34318,7 @@
         <v>6.9399810190854339E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="F31" s="1" t="s">
         <v>62</v>
       </c>
@@ -34327,7 +34326,7 @@
         <v>6.14708926222515E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18">
       <c r="F32" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>